<commit_message>
epbc changes in 2024 map
</commit_message>
<xml_diff>
--- a/data/epbc_changes_since2023_2024.xlsx
+++ b/data/epbc_changes_since2023_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shosh\OneDrive\2 PhD\GIT\ausenv-biodiversity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A5D2D-3993-4F51-95FC-04C9DE633A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E019F-0BB2-4A9C-BAED-977FF80CEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2865" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6AD6BC80-5F58-4D4F-9588-9DC886987F73}"/>
+    <workbookView xWindow="28680" yWindow="-2865" windowWidth="29040" windowHeight="15720" xr2:uid="{6AD6BC80-5F58-4D4F-9588-9DC886987F73}"/>
   </bookViews>
   <sheets>
     <sheet name="changes" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
   <si>
     <t>Species</t>
   </si>
@@ -439,13 +439,16 @@
   </si>
   <si>
     <t>Southern Bluefin Tuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population increase since 2000s due to fishery management result in species no longer being eligible under the 5 categories for EPBC listing. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +471,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -489,11 +498,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A070516-4839-4340-82F2-DBF7ECE9F6BF}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1839,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBB87A3-85C7-420D-AF3E-575A3FEED9B4}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1880,7 +1890,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.5">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1898,6 +1908,9 @@
       </c>
       <c r="F2" t="s">
         <v>130</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>